<commit_message>
Add new data and update accused list
</commit_message>
<xml_diff>
--- a/京華城被告.xlsx
+++ b/京華城被告.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="113">
   <si>
     <t xml:space="preserve">姓名</t>
   </si>
@@ -64,6 +65,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">前</t>
     </r>
@@ -73,6 +75,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">臺北市市長</t>
     </r>
@@ -81,6 +84,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -98,6 +102,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－</t>
     </r>
@@ -115,6 +120,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）
 </t>
@@ -125,6 +131,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">台灣民眾黨主席</t>
     </r>
@@ -133,6 +140,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -150,6 +158,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－）</t>
     </r>
@@ -160,6 +169,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">被告</t>
     </r>
@@ -177,6 +187,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">羈押禁見</t>
     </r>
@@ -193,6 +204,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">前</t>
     </r>
@@ -202,6 +214,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">臺北市政府工務局</t>
     </r>
@@ -210,6 +223,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">局長（</t>
     </r>
@@ -227,6 +241,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－</t>
     </r>
@@ -244,6 +259,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）
 前臺北市副市長兼任</t>
@@ -254,6 +270,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">臺北市都市計畫委員會</t>
     </r>
@@ -262,6 +279,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主任委員（</t>
     </r>
@@ -279,6 +297,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－</t>
     </r>
@@ -296,6 +315,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -310,6 +330,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">臺北市議員</t>
     </r>
@@ -318,6 +339,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -335,6 +357,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－）
 前</t>
@@ -345,6 +368,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">中國國民黨中央常務委員</t>
     </r>
@@ -353,6 +377,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -370,6 +395,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－</t>
     </r>
@@ -387,6 +413,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -410,6 +437,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">威京集團子公司受薪顧問、應曉薇助理
 曾任</t>
@@ -420,6 +448,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">臺北市政府都市發展局</t>
     </r>
@@ -428,6 +457,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">副總工程司</t>
     </r>
@@ -451,6 +481,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">威京總部集團主席
 前</t>
@@ -461,6 +492,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">中國國民黨</t>
     </r>
@@ -469,6 +501,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">中央常務委員（</t>
     </r>
@@ -486,6 +519,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－</t>
     </r>
@@ -503,6 +537,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -522,6 +557,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">註 </t>
     </r>
@@ -552,6 +588,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">郝龍斌市府</t>
     </r>
@@ -560,6 +597,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">時期任</t>
     </r>
@@ -569,6 +607,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">臺北市政府兵役局</t>
     </r>
@@ -577,6 +616,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">局長（</t>
     </r>
@@ -594,6 +634,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－</t>
     </r>
@@ -611,6 +652,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）
 後擔任威京集團子公司鼎越開發董事長，與本案相關人士關係密切（認罪、坦承行賄）</t>
@@ -628,6 +670,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">被告</t>
     </r>
@@ -645,6 +688,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">萬元交保</t>
     </r>
@@ -658,6 +702,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">應曉薇男友、應曉薇議員辦公室執行長，</t>
     </r>
@@ -667,6 +712,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">松聯幫</t>
     </r>
@@ -675,6 +721,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">前堂主</t>
     </r>
@@ -695,6 +742,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">被告</t>
     </r>
@@ -712,6 +760,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">萬元交保</t>
     </r>
@@ -734,6 +783,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">被告</t>
     </r>
@@ -751,6 +801,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">萬元交保</t>
     </r>
@@ -767,6 +818,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">被告</t>
     </r>
@@ -784,6 +836,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">萬元交保</t>
     </r>
@@ -800,6 +853,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">被告</t>
     </r>
@@ -817,6 +871,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">萬元交保</t>
     </r>
@@ -833,6 +888,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">被告</t>
     </r>
@@ -850,6 +906,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">限制住居</t>
     </r>
@@ -866,6 +923,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">被告</t>
     </r>
@@ -883,6 +941,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">無保請回</t>
     </r>
@@ -923,6 +982,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">前</t>
     </r>
@@ -932,6 +992,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">第一夫人周美青</t>
     </r>
@@ -940,6 +1001,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">之同學，受</t>
     </r>
@@ -949,6 +1011,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">馬英九前總統</t>
     </r>
@@ -957,6 +1020,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">提名擔任</t>
     </r>
@@ -966,6 +1030,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">監察委員</t>
     </r>
@@ -974,6 +1039,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -991,6 +1057,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－</t>
     </r>
@@ -1008,6 +1075,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）
 被指控施壓市府，卸任監委後於威京集團旗下沈春池文教基金會任董事</t>
@@ -1035,6 +1103,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">威京集團關係企業「中華工程」董事長</t>
     </r>
@@ -1044,6 +1113,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">沈慶京</t>
     </r>
@@ -1052,6 +1122,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">特助</t>
     </r>
@@ -1072,6 +1143,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">柯文哲市府臺北市政府都市發展局</t>
     </r>
@@ -1080,6 +1152,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">局長（</t>
     </r>
@@ -1097,6 +1170,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－</t>
     </r>
@@ -1114,6 +1188,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）
 </t>
@@ -1124,6 +1199,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">蔣萬安市府臺北市政府工務局</t>
     </r>
@@ -1132,6 +1208,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">局長（</t>
     </r>
@@ -1149,12 +1226,175 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">－）</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">嫌犯</t>
+  </si>
+  <si>
+    <t xml:space="preserve">王令麟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森集團總裁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">證人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">邱佩琳</t>
+  </si>
+  <si>
+    <t xml:space="preserve">基隆市副市長</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陳盈助</t>
+  </si>
+  <si>
+    <t xml:space="preserve">博弈教父</t>
+  </si>
+  <si>
+    <t xml:space="preserve">張高祥</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森電視總裁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">謝明珠</t>
+  </si>
+  <si>
+    <t xml:space="preserve">前台北市長辦公室主任</t>
+  </si>
+  <si>
+    <t xml:space="preserve">許芷瑜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">橘子</t>
+  </si>
+  <si>
+    <t xml:space="preserve">林建民</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森財易購財務經理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">未傳訊</t>
+  </si>
+  <si>
+    <t xml:space="preserve">楊愷崴</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森寵物資深協理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">趙世亨</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森直銷電商總經理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">彭鴻珷</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森購物經理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">林元中</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森購物協理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">王霞雲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森集團法務部經理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">理致琳</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森保貸總經理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">林宜嬪</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森財易購出納</t>
+  </si>
+  <si>
+    <t xml:space="preserve">張曉萍</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森國際</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蔡靜麗</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森集團人資行政部襄理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">廖尚文</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森國際董事長</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陳世志</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森國際董事</t>
+  </si>
+  <si>
+    <t xml:space="preserve">繆文強</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森歡樂旅行社</t>
+  </si>
+  <si>
+    <t xml:space="preserve">李美燕</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森集團</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宋湘嵐</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森購物執行長</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蔡高明</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森房屋董事長</t>
+  </si>
+  <si>
+    <t xml:space="preserve">林晉祥</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森集團人資行政部資深協理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">徐永亮</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森購物副總經理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陳雅惠</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東森集團副理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">捐贈者／支出對象</t>
+  </si>
+  <si>
+    <t xml:space="preserve">傳訊身份</t>
   </si>
 </sst>
 </file>
@@ -1193,12 +1433,6 @@
       <sz val="10"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1213,11 +1447,13 @@
       <color rgb="FF0000FF"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1231,6 +1467,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1275,7 +1516,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1288,27 +1529,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1329,10 +1582,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1712,6 +1965,281 @@
       <c r="C24" s="8"/>
       <c r="E24" s="7" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1751,4 +2279,599 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="83.9"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="柯文哲"/>
+    <hyperlink ref="A3" r:id="rId2" display="彭振聲"/>
+    <hyperlink ref="A4" r:id="rId3" display="應曉薇"/>
+    <hyperlink ref="A5" r:id="rId4" display="吳順民"/>
+    <hyperlink ref="A6" r:id="rId5" display="沈慶京"/>
+    <hyperlink ref="A7" r:id="rId6" display="李文宗"/>
+    <hyperlink ref="B7" r:id="rId7" display="柯文哲市府時期任台北市長辦公室主任（2018－2019）台北捷運公司董事長（2019－2023）"/>
+    <hyperlink ref="A8" r:id="rId8" display="朱亞虎"/>
+    <hyperlink ref="A9" r:id="rId9" display="陳玉坤"/>
+    <hyperlink ref="A10" r:id="rId10" display="王尊侃"/>
+    <hyperlink ref="A11" r:id="rId11" display="黃景茂"/>
+    <hyperlink ref="B11" r:id="rId12" display="柯文哲市府時期任都發局局長（2018－2021）"/>
+    <hyperlink ref="A12" r:id="rId13" display="張志澄"/>
+    <hyperlink ref="A13" r:id="rId14" display="陳佳敏"/>
+    <hyperlink ref="A14" r:id="rId15" display="陳俊源"/>
+    <hyperlink ref="A15" r:id="rId16" display="邵琇珮"/>
+    <hyperlink ref="B15" r:id="rId17" display="臺北市政府都市發展局總工程司暨臺北市都市計畫委員會執行秘書"/>
+    <hyperlink ref="A16" r:id="rId18" display="童中白"/>
+    <hyperlink ref="B16" r:id="rId19" location="cite_note-19" display="沈春池文教基金會前秘書長[18]"/>
+    <hyperlink ref="A17" r:id="rId20" display="黃淑雯"/>
+    <hyperlink ref="A18" r:id="rId21" display="洪秀鳳"/>
+    <hyperlink ref="A19" r:id="rId22" display="范雅琪"/>
+    <hyperlink ref="A20" r:id="rId23" display="陳秀桃"/>
+    <hyperlink ref="A21" r:id="rId24" display="劉芷安"/>
+    <hyperlink ref="A22" r:id="rId25" display="孫鳳群"/>
+    <hyperlink ref="A23" r:id="rId26" display="劉德勳"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>